<commit_message>
Wersja przed końcowa. Do poprawienia eksport do html.
</commit_message>
<xml_diff>
--- a/Pomiary_SYS_DIA.xlsx
+++ b/Pomiary_SYS_DIA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\PycharmProjects\blood_pressure_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A916027-64F7-40A6-8D68-69927858AC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04189F81-6C24-41FF-AA94-50741127548B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12204" yWindow="3588" windowWidth="18192" windowHeight="11328" xr2:uid="{8ECF50D0-7F8A-44A1-A98D-A72B22A3D8F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{8ECF50D0-7F8A-44A1-A98D-A72B22A3D8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -477,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E7332D-E79A-473A-84F2-EAE1ACC73729}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="G125" sqref="G125"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2546,6 +2546,125 @@
         <v>86</v>
       </c>
     </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="10">
+        <v>45973</v>
+      </c>
+      <c r="B122" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C122" s="2">
+        <v>109</v>
+      </c>
+      <c r="D122" s="2">
+        <v>65</v>
+      </c>
+      <c r="E122" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="10">
+        <v>45973</v>
+      </c>
+      <c r="B123" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C123" s="2">
+        <v>112</v>
+      </c>
+      <c r="D123" s="2">
+        <v>63</v>
+      </c>
+      <c r="E123" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="10">
+        <v>45973</v>
+      </c>
+      <c r="B124" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C124" s="2">
+        <v>116</v>
+      </c>
+      <c r="D124" s="2">
+        <v>75</v>
+      </c>
+      <c r="E124" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="10">
+        <v>45973</v>
+      </c>
+      <c r="B125" s="5">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C125" s="2">
+        <v>114</v>
+      </c>
+      <c r="D125" s="2">
+        <v>69</v>
+      </c>
+      <c r="E125" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="10">
+        <v>45974</v>
+      </c>
+      <c r="B126" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C126" s="2">
+        <v>101</v>
+      </c>
+      <c r="D126" s="2">
+        <v>63</v>
+      </c>
+      <c r="E126" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="10">
+        <v>45974</v>
+      </c>
+      <c r="B127" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C127" s="2">
+        <v>112</v>
+      </c>
+      <c r="D127" s="2">
+        <v>60</v>
+      </c>
+      <c r="E127" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="10">
+        <v>45974</v>
+      </c>
+      <c r="B128" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C128" s="2">
+        <v>106</v>
+      </c>
+      <c r="D128" s="2">
+        <v>65</v>
+      </c>
+      <c r="E128" s="2">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E60" xr:uid="{54E7332D-E79A-473A-84F2-EAE1ACC73729}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>